<commit_message>
using mechanicalsoup instead of selenium
</commit_message>
<xml_diff>
--- a/workspace/code/analyzer/file_processing/template/excel_format.xlsx
+++ b/workspace/code/analyzer/file_processing/template/excel_format.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Stock market investment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_20f9\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D8C00301-D5A2-495A-878D-7B4F74450377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAF04FDD-7096-4ED6-92AD-3D354BE20B1E}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{400D316A-83E7-45D6-AA0A-7DCDB78DFA50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{557F4819-B8B0-463E-B870-CE92581E9C0A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BD4D62F-CA13-407D-B30F-E9A78808E7C9}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{8BD4D62F-CA13-407D-B30F-E9A78808E7C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
-    <sheet name="Quarterly" sheetId="2" r:id="rId2"/>
+    <sheet name="Notes" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Yearly!$A$5:$BU$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Yearly!$A$5:$CZ$5</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
   <si>
     <t>Sales = Revenue</t>
   </si>
@@ -63,67 +63,169 @@
     <t>Group</t>
   </si>
   <si>
+    <t>Market Cap</t>
+  </si>
+  <si>
     <t>CMP</t>
   </si>
   <si>
     <t>Valuation</t>
   </si>
   <si>
-    <t>Current P/E</t>
+    <t>PEG</t>
+  </si>
+  <si>
+    <t>Current P/E(x)</t>
   </si>
   <si>
     <t>Avg PE (5 yrs)</t>
   </si>
   <si>
-    <t>PEG</t>
-  </si>
-  <si>
     <t>EPS</t>
   </si>
   <si>
-    <t>EPS CAGR(3 yrs)</t>
-  </si>
-  <si>
-    <t>ROE</t>
-  </si>
-  <si>
-    <t>ROCE</t>
+    <t>EPS CAGR %(3 yrs)</t>
+  </si>
+  <si>
+    <t>ROE(%)</t>
+  </si>
+  <si>
+    <t>ROCE(%)</t>
+  </si>
+  <si>
+    <t>P/B(x)</t>
+  </si>
+  <si>
+    <t>Dividend Yield</t>
+  </si>
+  <si>
+    <t>Debt to equity ratio</t>
+  </si>
+  <si>
+    <t>Interest Coverage Ratios</t>
+  </si>
+  <si>
+    <t>Revenue CAGR(3 yrs)</t>
+  </si>
+  <si>
+    <t>Profit CAGR(3 yrs)</t>
+  </si>
+  <si>
+    <t>Net Profit CAGR(3 yrs)</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>Net Cash Flow</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>Companies can alter profit and sales figures. So the priority should not be on profit and sales growth figures</t>
+  </si>
+  <si>
+    <t>Find companies that have economic moat during early stages</t>
+  </si>
+  <si>
+    <t>Aviod companies that is having debt to equity ratio more than 1 and (increasing)</t>
+  </si>
+  <si>
+    <t>Avoid companies having ROE less than 12% and( decreasing over years)</t>
+  </si>
+  <si>
+    <t>Better to invest in companies where promotors holding is increasing</t>
+  </si>
+  <si>
+    <t>Better to invest in companies where FIIs stake is increasing</t>
+  </si>
+  <si>
+    <t>Avoid companies where retail investors stake is increasing, sign of FIIs and DIIs stake decrease and early sign of meltdown of company</t>
+  </si>
+  <si>
+    <t>Pledging of shares 2-8% is fine but keep an eye on it if it is increasing</t>
+  </si>
+  <si>
+    <t>Aviod companies where promotors pledge more than 30% of the holdings and the pledged percentage is increasing</t>
+  </si>
+  <si>
+    <t>Good companies provide dividend from past 10-20 yrs, signifies good balance sheet</t>
+  </si>
+  <si>
+    <t>Tax should match 30%-35% of profit otherwise dig deeper</t>
+  </si>
+  <si>
+    <t>avg ROE for past 5 yrs should be &gt;=20%</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>Compare with its historical average and if its trading less than its historical avg P/E could be a buy</t>
+  </si>
+  <si>
+    <t>Compare with its peers</t>
+  </si>
+  <si>
+    <t>Compare with sensex</t>
+  </si>
+  <si>
+    <t>higher growth higher PE</t>
+  </si>
+  <si>
+    <t>Massive cashflow and less leveraged</t>
   </si>
   <si>
     <t>P/B</t>
   </si>
   <si>
-    <t>Dividend Yield</t>
-  </si>
-  <si>
-    <t>Debt to equity ratio</t>
-  </si>
-  <si>
-    <t>Interest Coverage Ratios</t>
-  </si>
-  <si>
-    <t>Revenue CAGR</t>
-  </si>
-  <si>
-    <t>Profit CAGR</t>
-  </si>
-  <si>
-    <t>Net Profit CAGR</t>
-  </si>
-  <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>Net Profit</t>
-  </si>
-  <si>
-    <t>Net Cash Flow</t>
-  </si>
-  <si>
-    <t>Same structure as yearly</t>
+    <t>Lower the P/B the better</t>
+  </si>
+  <si>
+    <t>Current PE is not more than two times of the last three years average earnings growth rate</t>
+  </si>
+  <si>
+    <t>PEG = PE/Earning growth rate</t>
+  </si>
+  <si>
+    <t>PEG is calculated for past 3yrs</t>
+  </si>
+  <si>
+    <t>PEG&lt;0.5</t>
+  </si>
+  <si>
+    <t>undervalued and could be an opportunity</t>
+  </si>
+  <si>
+    <t>0.5&lt;PEG&lt;1</t>
+  </si>
+  <si>
+    <t>undervalued or resonably valued</t>
+  </si>
+  <si>
+    <t>1&lt;PEG&lt;2</t>
+  </si>
+  <si>
+    <t>Reasonably valued</t>
+  </si>
+  <si>
+    <t>PEG&gt;2</t>
+  </si>
+  <si>
+    <t>Over valued</t>
+  </si>
+  <si>
+    <t>Calculated for past 5 yrs</t>
   </si>
 </sst>
 </file>
@@ -239,6 +341,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,9 +349,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4B59EE-406E-4588-820C-A407EF25A70E}">
-  <dimension ref="A1:BV52"/>
+  <dimension ref="A1:CZ25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:BV7"/>
+      <selection activeCell="DB10" sqref="A6:DB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -576,103 +676,135 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="14.28515625" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" customWidth="1"/>
+    <col min="23" max="23" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="6.42578125" customWidth="1"/>
+    <col min="28" max="28" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" customWidth="1"/>
+    <col min="30" max="30" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="8" customWidth="1"/>
     <col min="35" max="35" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" customWidth="1"/>
+    <col min="37" max="37" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.28515625" customWidth="1"/>
+    <col min="41" max="41" width="6" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.28515625" customWidth="1"/>
     <col min="44" max="44" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.85546875" customWidth="1"/>
+    <col min="48" max="48" width="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.28515625" customWidth="1"/>
+    <col min="51" max="51" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8" customWidth="1"/>
+    <col min="55" max="55" width="7" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.28515625" customWidth="1"/>
+    <col min="58" max="58" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="7.7109375" customWidth="1"/>
+    <col min="62" max="62" width="7.42578125" customWidth="1"/>
     <col min="63" max="63" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" customWidth="1"/>
+    <col min="65" max="65" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="7.85546875" customWidth="1"/>
+    <col min="69" max="69" width="5.85546875" customWidth="1"/>
+    <col min="70" max="70" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.28515625" customWidth="1"/>
     <col min="72" max="72" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7" customWidth="1"/>
+    <col min="76" max="76" width="7.5703125" customWidth="1"/>
+    <col min="77" max="77" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="8.28515625" customWidth="1"/>
+    <col min="79" max="79" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="7.5703125" customWidth="1"/>
+    <col min="83" max="83" width="6.7109375" customWidth="1"/>
+    <col min="84" max="84" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="8.28515625" customWidth="1"/>
+    <col min="86" max="86" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.140625" customWidth="1"/>
+    <col min="90" max="90" width="7" customWidth="1"/>
+    <col min="91" max="91" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8.28515625" customWidth="1"/>
+    <col min="93" max="93" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="7.28515625" customWidth="1"/>
+    <col min="97" max="97" width="6.7109375" customWidth="1"/>
+    <col min="98" max="98" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="8.28515625" customWidth="1"/>
+    <col min="100" max="100" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8" customWidth="1"/>
+    <col min="104" max="104" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74">
+    <row r="1" spans="1:104" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:74">
+    <row r="2" spans="1:104" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
+      <c r="U2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:74">
+    <row r="3" spans="1:104" ht="15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:74">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:104" ht="15">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -689,100 +821,127 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="6">
+      <c r="U4" s="7">
         <v>2020</v>
       </c>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
-      <c r="AA4" s="6">
-        <f>W4-1</f>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="7">
+        <f>U4-1</f>
         <v>2019</v>
       </c>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
+      <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="6">
-        <f>AA4-1</f>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="7">
+        <f>AB4-1</f>
         <v>2018</v>
       </c>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="6">
-        <f>AE4-1</f>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="7">
+        <f>AI4-1</f>
         <v>2017</v>
       </c>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="6">
-        <f>AI4-1</f>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="9"/>
+      <c r="AW4" s="7">
+        <f>AP4-1</f>
         <v>2016</v>
       </c>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="6">
-        <f t="shared" ref="AQ4" si="0">AM4-1</f>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="9"/>
+      <c r="BD4" s="7">
+        <f t="shared" ref="BD4" si="0">AW4-1</f>
         <v>2015</v>
       </c>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="8"/>
-      <c r="AU4" s="6">
-        <f t="shared" ref="AU4" si="1">AQ4-1</f>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+      <c r="BG4" s="8"/>
+      <c r="BH4" s="8"/>
+      <c r="BI4" s="8"/>
+      <c r="BJ4" s="9"/>
+      <c r="BK4" s="7">
+        <f t="shared" ref="BK4" si="1">BD4-1</f>
         <v>2014</v>
       </c>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="8"/>
-      <c r="AY4" s="6">
-        <f t="shared" ref="AY4" si="2">AU4-1</f>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8"/>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="9"/>
+      <c r="BR4" s="7">
+        <f t="shared" ref="BR4" si="2">BK4-1</f>
         <v>2013</v>
       </c>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="8"/>
-      <c r="BC4" s="6">
-        <f t="shared" ref="BC4" si="3">AY4-1</f>
+      <c r="BS4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BU4" s="8"/>
+      <c r="BV4" s="8"/>
+      <c r="BW4" s="8"/>
+      <c r="BX4" s="9"/>
+      <c r="BY4" s="7">
+        <f t="shared" ref="BY4" si="3">BR4-1</f>
         <v>2012</v>
       </c>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="7"/>
-      <c r="BF4" s="8"/>
-      <c r="BG4" s="6">
-        <f t="shared" ref="BG4" si="4">BC4-1</f>
+      <c r="BZ4" s="8"/>
+      <c r="CA4" s="8"/>
+      <c r="CB4" s="8"/>
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="9"/>
+      <c r="CF4" s="7">
+        <f t="shared" ref="CF4" si="4">BY4-1</f>
         <v>2011</v>
       </c>
-      <c r="BH4" s="7"/>
-      <c r="BI4" s="7"/>
-      <c r="BJ4" s="8"/>
-      <c r="BK4" s="6">
-        <f t="shared" ref="BK4" si="5">BG4-1</f>
+      <c r="CG4" s="8"/>
+      <c r="CH4" s="8"/>
+      <c r="CI4" s="8"/>
+      <c r="CJ4" s="8"/>
+      <c r="CK4" s="8"/>
+      <c r="CL4" s="9"/>
+      <c r="CM4" s="7">
+        <f t="shared" ref="CM4" si="5">CF4-1</f>
         <v>2010</v>
       </c>
-      <c r="BL4" s="7"/>
-      <c r="BM4" s="7"/>
-      <c r="BN4" s="8"/>
-      <c r="BO4" s="6">
-        <f t="shared" ref="BO4" si="6">BK4-1</f>
+      <c r="CN4" s="8"/>
+      <c r="CO4" s="8"/>
+      <c r="CP4" s="8"/>
+      <c r="CQ4" s="8"/>
+      <c r="CR4" s="8"/>
+      <c r="CS4" s="9"/>
+      <c r="CT4" s="7">
+        <f t="shared" ref="CT4" si="6">CM4-1</f>
         <v>2009</v>
       </c>
-      <c r="BP4" s="7"/>
-      <c r="BQ4" s="7"/>
-      <c r="BR4" s="8"/>
-      <c r="BS4" s="9">
-        <f t="shared" ref="BS4" si="7">BO4-1</f>
-        <v>2008</v>
-      </c>
-      <c r="BT4" s="9"/>
-      <c r="BU4" s="9"/>
-      <c r="BV4" s="9"/>
-    </row>
-    <row r="5" spans="1:74">
+      <c r="CU4" s="8"/>
+      <c r="CV4" s="8"/>
+      <c r="CW4" s="8"/>
+      <c r="CX4" s="8"/>
+      <c r="CY4" s="8"/>
+      <c r="CZ4" s="9"/>
+    </row>
+    <row r="5" spans="1:104" ht="15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -840,23 +999,29 @@
       <c r="S5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="W5" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>25</v>
@@ -868,79 +1033,79 @@
         <v>27</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AF5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AJ5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AK5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AI5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AL5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AK5" s="2" t="s">
+      <c r="AQ5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AR5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AM5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AN5" s="2" t="s">
+      <c r="AS5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AO5" s="2" t="s">
+      <c r="AX5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AP5" s="2" t="s">
+      <c r="AY5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AQ5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AR5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AS5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AT5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AV5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AW5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AX5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AY5" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="AZ5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="BA5" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="BB5" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="BC5" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="BD5" s="2" t="s">
         <v>25</v>
@@ -952,107 +1117,433 @@
         <v>27</v>
       </c>
       <c r="BG5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BH5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BI5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BJ5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BK5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BI5" s="2" t="s">
+      <c r="BL5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BJ5" s="2" t="s">
+      <c r="BM5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="BK5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="BL5" s="2" t="s">
+      <c r="BN5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BO5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BR5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BM5" s="2" t="s">
+      <c r="BS5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BN5" s="2" t="s">
+      <c r="BT5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="BO5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="BP5" s="2" t="s">
+      <c r="BU5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BV5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BW5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BX5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BY5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BQ5" s="2" t="s">
+      <c r="BZ5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BR5" s="2" t="s">
+      <c r="CA5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="BS5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="BT5" s="2" t="s">
+      <c r="CB5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CC5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CD5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CE5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="CF5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BU5" s="2" t="s">
+      <c r="CG5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BV5" s="2" t="s">
+      <c r="CH5" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:74">
-      <c r="N11" s="3"/>
-    </row>
-    <row r="13" spans="1:74">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:74">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:74">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
+      <c r="CI5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CJ5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CK5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CL5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="CM5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="CN5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="CO5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="CP5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CQ5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CR5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CS5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="CT5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="CU5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="CV5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="CW5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CX5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CY5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="CZ5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:104" ht="15"/>
+    <row r="7" spans="1:104" ht="15"/>
+    <row r="8" spans="1:104" ht="15"/>
+    <row r="9" spans="1:104" ht="15"/>
+    <row r="10" spans="1:104" ht="15"/>
+    <row r="11" spans="1:104" ht="15">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:104" ht="15">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+    </row>
+    <row r="13" spans="1:104" ht="15">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+    </row>
+    <row r="14" spans="1:104" ht="15">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" spans="1:104" ht="15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:104" ht="15">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="1:16" ht="15">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="1:16" ht="15">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="1:16" ht="15">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" ht="15">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="1:16" ht="15">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="1:16" ht="15">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="1:16" ht="15">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" ht="15">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+    </row>
+    <row r="25" spans="1:16" ht="15">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="AI4:AL4"/>
-    <mergeCell ref="BS4:BV4"/>
-    <mergeCell ref="AM4:AP4"/>
-    <mergeCell ref="AQ4:AT4"/>
-    <mergeCell ref="AU4:AX4"/>
-    <mergeCell ref="AY4:BB4"/>
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BG4:BJ4"/>
-    <mergeCell ref="BK4:BN4"/>
-    <mergeCell ref="BO4:BR4"/>
+  <mergeCells count="12">
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="BD4:BJ4"/>
+    <mergeCell ref="CT4:CZ4"/>
+    <mergeCell ref="BK4:BQ4"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BY4:CE4"/>
+    <mergeCell ref="CF4:CL4"/>
+    <mergeCell ref="CM4:CS4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1060,18 +1551,183 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5305BE95-5EE1-4941-B2D1-E4D6EFB1B193}">
-  <dimension ref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E67B9C-522D-401F-B358-8706AC720DD0}">
+  <dimension ref="A3:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>28</v>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" ht="15">
+      <c r="A17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="15">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15">
+      <c r="A23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" ht="15">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="L29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="L35" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>